<commit_message>
feat: fix some bugs, add multi-ticker backtest, dynamic strategy import, and persistent results appending
</commit_message>
<xml_diff>
--- a/strategies_results.xlsx
+++ b/strategies_results.xlsx
@@ -1,43 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AAPL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="MSFT" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,26 +46,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +399,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>equity_curve</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>final_value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_return</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>max_drawdown</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>sharpe</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trade_count</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>win_rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>avg_win</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>avg_loss</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>profit_factor</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>strategy_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Date
+2022-01-03    100000.000000
+2022-01-04    100000.000000
+2022-01-05    100000.000000
+2022-01-06    100000.000000
+2022-01-07    100000.000000
+                  ...      
+2023-12-22    108779.741026
+2023-12-26    108470.705610
+2023-12-27    108526.885231
+2023-12-28    108768.496466
+2023-12-29    108178.519762
+Length: 501, dtype: float64</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>108178.5197621365</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.08178519762136482</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.2391994334562445</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.3145575745934971</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27.49614715576172</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-6.890348434448242</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.9976326820533106</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>example_ema_crossover</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>equity_curve</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>final_value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_return</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>max_drawdown</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>sharpe</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trade_count</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>win_rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>avg_win</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>avg_loss</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>profit_factor</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>strategy_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Date
+2022-01-03    100000.000000
+2022-01-04    100000.000000
+2022-01-05    100000.000000
+2022-01-06    100000.000000
+2022-01-07    100000.000000
+                  ...      
+2023-12-22    110826.784276
+2023-12-26    110850.462809
+2023-12-27    110675.900975
+2023-12-28    111033.900668
+2023-12-29    111258.759979
+Length: 501, dtype: float64</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>111258.7599792535</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1125875997925352</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.2880248272734179</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.3685697719438401</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>41.39932250976562</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-10.47931480407715</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.9876438317717715</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>example_ema_crossover</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: make strategy function detection robust for all strategies
</commit_message>
<xml_diff>
--- a/strategies_results.xlsx
+++ b/strategies_results.xlsx
@@ -2,16 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="AAPL" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MSFT" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="AAPL" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MSFT" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -20,7 +21,7 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -63,9 +64,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -148,44 +149,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -212,15 +213,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -247,7 +247,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -259,142 +258,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -404,15 +427,124 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>equity_curve</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>final_value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_return</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>max_drawdown</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>sharpe</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trade_count</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>win_rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>avg_win</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>avg_loss</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>profit_factor</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>strategy_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Date
+2022-01-03    100000.000000
+2022-01-04    100000.000000
+2022-01-05    100000.000000
+2022-01-06    100000.000000
+2022-01-07    100000.000000
+                  ...      
+2023-12-22    108779.618247
+2023-12-26    108470.591816
+2023-12-27    108526.762737
+2023-12-28    108768.373699
+2023-12-29    108178.397661
+Length: 501, dtype: float64</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>108178.3976614393</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.08178397661439285</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.2391994999516704</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.3145542179576449</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27.49613952636719</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-6.890371322631836</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.9976290913399135</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>example_ema_crossover</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -497,25 +629,25 @@
 2022-01-06    100000.000000
 2022-01-07    100000.000000
                   ...      
-2023-12-22    108779.741026
-2023-12-26    108470.705610
-2023-12-27    108526.885231
-2023-12-28    108768.496466
-2023-12-29    108178.519762
+2023-12-22    110826.873309
+2023-12-26    110850.542727
+2023-12-27    110675.980768
+2023-12-28    111033.971587
+2023-12-29    111258.831061
 Length: 501, dtype: float64</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>108178.5197621365</v>
+        <v>111258.8310607065</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08178519762136482</v>
+        <v>0.1125883106070653</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2391994334562445</v>
+        <v>-0.2880242813881386</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3145575745934971</v>
+        <v>0.3685714379404278</v>
       </c>
       <c r="F2" t="n">
         <v>10</v>
@@ -524,13 +656,13 @@
         <v>0.2</v>
       </c>
       <c r="H2" t="n">
-        <v>27.49614715576172</v>
+        <v>41.39935302734375</v>
       </c>
       <c r="I2" t="n">
-        <v>-6.890348434448242</v>
+        <v>-10.47929573059082</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9976326820533106</v>
+        <v>0.9876463574382223</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -549,123 +681,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>equity_curve</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>final_value</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>total_return</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>max_drawdown</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>sharpe</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>trade_count</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>win_rate</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>avg_win</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>avg_loss</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>profit_factor</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>strategy_name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Date
-2022-01-03    100000.000000
-2022-01-04    100000.000000
-2022-01-05    100000.000000
-2022-01-06    100000.000000
-2022-01-07    100000.000000
-                  ...      
-2023-12-22    110826.784276
-2023-12-26    110850.462809
-2023-12-27    110675.900975
-2023-12-28    111033.900668
-2023-12-29    111258.759979
-Length: 501, dtype: float64</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>111258.7599792535</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1125875997925352</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.2880248272734179</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.3685697719438401</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H2" t="n">
-        <v>41.39932250976562</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-10.47931480407715</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.9876438317717715</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>example_ema_crossover</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>